<commit_message>
complete code and fisrt test
</commit_message>
<xml_diff>
--- a/sample_parameter.xlsx
+++ b/sample_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\term2\scm\final-project\SCM-finalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D958043-0FDA-4E7C-B072-3BFB765F6D30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EBAE74-483A-4D03-B300-8BE616FD7024}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -983,42 +983,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1515,10 +1515,10 @@
   <dimension ref="A8:AL73"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" ySplit="12" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="AI15" sqref="AI15"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1535,14 +1535,14 @@
   <sheetData>
     <row r="8" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:38" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="36"/>
     </row>
     <row r="11" spans="2:38" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="17"/>
@@ -1572,72 +1572,72 @@
       </c>
     </row>
     <row r="13" spans="2:38" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-      <c r="J13" s="44" t="s">
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="J13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="K13" s="44" t="s">
+      <c r="K13" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="M13" s="44" t="s">
+      <c r="M13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="N13" s="44" t="s">
+      <c r="N13" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="P13" s="44" t="s">
+      <c r="P13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="Q13" s="44" t="s">
+      <c r="Q13" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="S13" s="44" t="s">
+      <c r="S13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="T13" s="44" t="s">
+      <c r="T13" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="44" t="s">
+      <c r="V13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="W13" s="44" t="s">
+      <c r="W13" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="Y13" s="44" t="s">
+      <c r="Y13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="Z13" s="44" t="s">
+      <c r="Z13" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="AB13" s="44" t="s">
+      <c r="AB13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="AC13" s="44" t="s">
+      <c r="AC13" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="AE13" s="44" t="s">
+      <c r="AE13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="AF13" s="44" t="s">
+      <c r="AF13" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="AH13" s="44" t="s">
+      <c r="AH13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="AI13" s="44" t="s">
+      <c r="AI13" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="AK13" s="44" t="s">
+      <c r="AK13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="AL13" s="44" t="s">
+      <c r="AL13" s="33" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1676,64 +1676,64 @@
         <v>146</v>
       </c>
       <c r="G15" s="12"/>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="K15" s="44" t="s">
+      <c r="K15" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="M15" s="44" t="s">
+      <c r="M15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="N15" s="44" t="s">
+      <c r="N15" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="P15" s="44" t="s">
+      <c r="P15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="Q15" s="44" t="s">
+      <c r="Q15" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="S15" s="44" t="s">
+      <c r="S15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="T15" s="44" t="s">
+      <c r="T15" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="V15" s="44" t="s">
+      <c r="V15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="W15" s="44" t="s">
+      <c r="W15" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="Y15" s="44" t="s">
+      <c r="Y15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="Z15" s="44" t="s">
+      <c r="Z15" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="AB15" s="44" t="s">
+      <c r="AB15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="AC15" s="44" t="s">
+      <c r="AC15" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="AE15" s="44" t="s">
+      <c r="AE15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="AF15" s="44" t="s">
+      <c r="AF15" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="AH15" s="44" t="s">
+      <c r="AH15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="AI15" s="44" t="s">
+      <c r="AI15" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="AK15" s="44" t="s">
+      <c r="AK15" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="AL15" s="44" t="s">
+      <c r="AL15" s="33" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1754,64 +1754,64 @@
         <v>122</v>
       </c>
       <c r="G16" s="12"/>
-      <c r="J16" s="44" t="s">
+      <c r="J16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="K16" s="44" t="s">
+      <c r="K16" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="M16" s="44" t="s">
+      <c r="M16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="N16" s="44" t="s">
+      <c r="N16" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="P16" s="44" t="s">
+      <c r="P16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="Q16" s="44" t="s">
+      <c r="Q16" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="S16" s="44" t="s">
+      <c r="S16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="T16" s="44" t="s">
+      <c r="T16" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="V16" s="44" t="s">
+      <c r="V16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="W16" s="44" t="s">
+      <c r="W16" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="Y16" s="44" t="s">
+      <c r="Y16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="Z16" s="44" t="s">
+      <c r="Z16" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AB16" s="44" t="s">
+      <c r="AB16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="AC16" s="44" t="s">
+      <c r="AC16" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="AE16" s="44" t="s">
+      <c r="AE16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="AF16" s="44" t="s">
+      <c r="AF16" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="AH16" s="44" t="s">
+      <c r="AH16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="AI16" s="44" t="s">
+      <c r="AI16" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="AK16" s="44" t="s">
+      <c r="AK16" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="AL16" s="44" t="s">
+      <c r="AL16" s="33" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1832,64 +1832,64 @@
         <v>121</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="K17" s="44" t="s">
+      <c r="K17" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="M17" s="44" t="s">
+      <c r="M17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="N17" s="44" t="s">
+      <c r="N17" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="P17" s="44" t="s">
+      <c r="P17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="Q17" s="44" t="s">
+      <c r="Q17" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="S17" s="44" t="s">
+      <c r="S17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="T17" s="44" t="s">
+      <c r="T17" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="V17" s="44" t="s">
+      <c r="V17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="W17" s="44" t="s">
+      <c r="W17" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="Y17" s="44" t="s">
+      <c r="Y17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="Z17" s="44" t="s">
+      <c r="Z17" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="AB17" s="44" t="s">
+      <c r="AB17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="AC17" s="44" t="s">
+      <c r="AC17" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="AE17" s="44" t="s">
+      <c r="AE17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="AF17" s="44" t="s">
+      <c r="AF17" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AH17" s="44" t="s">
+      <c r="AH17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="AI17" s="44" t="s">
+      <c r="AI17" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="AK17" s="44" t="s">
+      <c r="AK17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="AL17" s="44" t="s">
+      <c r="AL17" s="33" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1910,64 +1910,64 @@
         <v>126</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="J18" s="44" t="s">
+      <c r="J18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="K18" s="44" t="s">
+      <c r="K18" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="M18" s="44" t="s">
+      <c r="M18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="N18" s="44" t="s">
+      <c r="N18" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="P18" s="44" t="s">
+      <c r="P18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="Q18" s="44" t="s">
+      <c r="Q18" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="S18" s="44" t="s">
+      <c r="S18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="T18" s="44" t="s">
+      <c r="T18" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="V18" s="44" t="s">
+      <c r="V18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="W18" s="44" t="s">
+      <c r="W18" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="Y18" s="44" t="s">
+      <c r="Y18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="Z18" s="44" t="s">
+      <c r="Z18" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="AB18" s="44" t="s">
+      <c r="AB18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AC18" s="44" t="s">
+      <c r="AC18" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="AE18" s="44" t="s">
+      <c r="AE18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AF18" s="44" t="s">
+      <c r="AF18" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="AH18" s="44" t="s">
+      <c r="AH18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AI18" s="44" t="s">
+      <c r="AI18" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AK18" s="44" t="s">
+      <c r="AK18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="AL18" s="44" t="s">
+      <c r="AL18" s="33" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1988,64 +1988,64 @@
         <v>125</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="K19" s="44" t="s">
+      <c r="K19" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="M19" s="44" t="s">
+      <c r="M19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="N19" s="44" t="s">
+      <c r="N19" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="P19" s="44" t="s">
+      <c r="P19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="Q19" s="44" t="s">
+      <c r="Q19" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="S19" s="44" t="s">
+      <c r="S19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="T19" s="44" t="s">
+      <c r="T19" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="V19" s="44" t="s">
+      <c r="V19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="W19" s="44" t="s">
+      <c r="W19" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="Y19" s="44" t="s">
+      <c r="Y19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="Z19" s="44" t="s">
+      <c r="Z19" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="AB19" s="44" t="s">
+      <c r="AB19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AC19" s="44" t="s">
+      <c r="AC19" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="AE19" s="44" t="s">
+      <c r="AE19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AF19" s="44" t="s">
+      <c r="AF19" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="AH19" s="44" t="s">
+      <c r="AH19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AI19" s="44" t="s">
+      <c r="AI19" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="AK19" s="44" t="s">
+      <c r="AK19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="AL19" s="44" t="s">
+      <c r="AL19" s="33" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2178,7 +2178,7 @@
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="19">
         <v>15</v>
       </c>
@@ -2213,14 +2213,14 @@
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:38" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
       <c r="J29"/>
       <c r="K29"/>
     </row>
@@ -2685,14 +2685,14 @@
       <c r="K57"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="42"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="44"/>
     </row>
     <row r="59" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="22">

</xml_diff>